<commit_message>
fixed issue for KAISI upload Invoice , special string and removal  and also the order of the processing in submitButtonHandling.py file
</commit_message>
<xml_diff>
--- a/processed/YouWant_INV240610111_1.xlsx
+++ b/processed/YouWant_INV240610111_1.xlsx
@@ -476,18 +476,18 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
+          <t>SinglePrice</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
           <t>EnglishDescription</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>SinglePrice</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -515,21 +515,21 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>693-1286064278</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
+          <t>6931286064278</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
+        <v>2.07</v>
+      </c>
+      <c r="J2" t="inlineStr">
         <is>
           <t>Wolong- (Wuzi Scent) Old Stove Pot 138g</t>
         </is>
-      </c>
-      <c r="J2" t="n">
-        <v>62.04</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -557,21 +557,21 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>693-1286065268</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
+          <t>6931286065268</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>2.07</v>
+      </c>
+      <c r="J3" t="inlineStr">
         <is>
           <t>Wolong- (Ecstasy Spicy) Old Stove Pot 128g</t>
         </is>
-      </c>
-      <c r="J3" t="n">
-        <v>62.04</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -599,21 +599,21 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>697-1657871364</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
+          <t>6971657871364</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="J4" t="inlineStr">
         <is>
           <t>San Yuanze-Hawthorn pulp Beijing cakes 160g</t>
         </is>
-      </c>
-      <c r="J4" t="n">
-        <v>21</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -641,21 +641,21 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>690-2083815103</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
+          <t>6902083815103</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>1.54</v>
+      </c>
+      <c r="J5" t="inlineStr">
         <is>
           <t>Wahaha- (sugar-free) Dahongpao oolong tea 500ml</t>
         </is>
-      </c>
-      <c r="J5" t="n">
-        <v>23.1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -683,21 +683,21 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>690-2083815110</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
+          <t>6902083815110</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>1.54</v>
+      </c>
+      <c r="J6" t="inlineStr">
         <is>
           <t>Wahaha- (sugar-free) Zhengshan small breeding black tea 500ml</t>
         </is>
-      </c>
-      <c r="J6" t="n">
-        <v>23.1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -725,21 +725,21 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>690-2083815134</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
+          <t>6902083815134</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>1.54</v>
+      </c>
+      <c r="J7" t="inlineStr">
         <is>
           <t>Wahaha- (Sugar-free) Pu'er tea 500ml</t>
         </is>
-      </c>
-      <c r="J7" t="n">
-        <v>23.1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -767,21 +767,21 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>690-2083815127</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
+          <t>6902083815127</t>
+        </is>
+      </c>
+      <c r="I8" t="n">
+        <v>1.54</v>
+      </c>
+      <c r="J8" t="inlineStr">
         <is>
           <t>Wahaha- (sugar-free) jasmine tea 500ml</t>
         </is>
-      </c>
-      <c r="J8" t="n">
-        <v>23.1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.25</v>
+        <v>10</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -809,21 +809,21 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>692-6896705277</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
+          <t>6926896705277</t>
+        </is>
+      </c>
+      <c r="I9" t="n">
+        <v>6.72</v>
+      </c>
+      <c r="J9" t="inlineStr">
         <is>
           <t>Jixiangju-Crispy double bamboo shoot 106g</t>
         </is>
-      </c>
-      <c r="J9" t="n">
-        <v>268.8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -851,21 +851,21 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>690-9003200117</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
+          <t>6909003200117</t>
+        </is>
+      </c>
+      <c r="I10" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="J10" t="inlineStr">
         <is>
           <t>Cuckoo City-150g of tempeh</t>
         </is>
-      </c>
-      <c r="J10" t="n">
-        <v>11.31</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0.25</v>
+        <v>10</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -893,21 +893,21 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>690-7592001429</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
+          <t>6907592001429</t>
+        </is>
+      </c>
+      <c r="I11" t="n">
+        <v>4.25</v>
+      </c>
+      <c r="J11" t="inlineStr">
         <is>
           <t>Wang Zhihe-dried yellow sauce 180g</t>
         </is>
-      </c>
-      <c r="J11" t="n">
-        <v>170.08</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -935,21 +935,21 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>692-8002376630</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
+          <t>6928002376630</t>
+        </is>
+      </c>
+      <c r="I12" t="n">
+        <v>2.41</v>
+      </c>
+      <c r="J12" t="inlineStr">
         <is>
           <t>Gan Juyuan-pure brown sugar 300g</t>
         </is>
-      </c>
-      <c r="J12" t="n">
-        <v>57.75</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -977,21 +977,21 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>692-2507808597</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
+          <t>6922507808597</t>
+        </is>
+      </c>
+      <c r="I13" t="n">
+        <v>2.84</v>
+      </c>
+      <c r="J13" t="inlineStr">
         <is>
           <t>Chen Keming- (Egg) Refined Noodle 1000g</t>
         </is>
-      </c>
-      <c r="J13" t="n">
-        <v>42.53</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -1019,21 +1019,21 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>692-2507808580</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
+          <t>6922507808580</t>
+        </is>
+      </c>
+      <c r="I14" t="n">
+        <v>2.84</v>
+      </c>
+      <c r="J14" t="inlineStr">
         <is>
           <t>Chen Keming- (Jin Dao) Refined Noodle 1000g</t>
         </is>
-      </c>
-      <c r="J14" t="n">
-        <v>42.53</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -1059,21 +1059,21 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>692-0404395981</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
+          <t>6920404395981</t>
+        </is>
+      </c>
+      <c r="I15" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="J15" t="inlineStr">
         <is>
           <t>Nongfu Villa-California Ximei 70g</t>
         </is>
-      </c>
-      <c r="J15" t="n">
-        <v>2.73</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -1099,21 +1099,21 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>693-2419100474</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
+          <t>6932419100474</t>
+        </is>
+      </c>
+      <c r="I16" t="n">
+        <v>8.75</v>
+      </c>
+      <c r="J16" t="inlineStr">
         <is>
           <t>Shuangrong- (Rose Black Sugar) Guanyin Pavilion 220g</t>
         </is>
-      </c>
-      <c r="J16" t="n">
-        <v>210</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -1122,7 +1122,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>001. 伊藤园-原味烏龍茶 500ml</t>
+          <t>伊藤园-原味烏龍茶 500ml</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -1141,21 +1141,21 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>695-8959708208</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>001. Ito Garden-Original Oolong Tea 500ml</t>
-        </is>
-      </c>
-      <c r="J17" t="n">
-        <v>13.71</v>
+          <t>6958959708208</t>
+        </is>
+      </c>
+      <c r="I17" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>Ito Garden-Original oolong tea 500ml</t>
+        </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -1164,7 +1164,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>002. 伊藤园-無糖冷萃綠茶 600ml</t>
+          <t>伊藤园-無糖冷萃綠茶 600ml</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -1183,21 +1183,21 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>695-8959708246</t>
-        </is>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>002. Ito Garden-sugar-free cold green tea 600ml</t>
-        </is>
-      </c>
-      <c r="J18" t="n">
-        <v>13.76</v>
+          <t>6958959708246</t>
+        </is>
+      </c>
+      <c r="I18" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>Ito Garden-sugar-free cold green tea 600ml</t>
+        </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -1206,7 +1206,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>003. 白家-酸湯肥牛調料 160g</t>
+          <t>白家-酸湯肥牛調料 160g</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -1225,21 +1225,21 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>697-4142070525</t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>003. Baijia-Sour soup fat beef seasoning 160g</t>
-        </is>
-      </c>
-      <c r="J19" t="n">
-        <v>72.45</v>
+          <t>6974142070525</t>
+        </is>
+      </c>
+      <c r="I19" t="n">
+        <v>2.42</v>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Baijia-Sour soup Fat beef seasoning 160g</t>
+        </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -1248,7 +1248,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>004. 白家-老鹵汁調料 120g</t>
+          <t>白家-老鹵汁調料 120g</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -1267,21 +1267,21 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>692-6410335416</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>004. Baijia-Old marinade seasoning 120g</t>
-        </is>
-      </c>
-      <c r="J20" t="n">
-        <v>56.7</v>
+          <t>6926410335416</t>
+        </is>
+      </c>
+      <c r="I20" t="n">
+        <v>1.89</v>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Baijia-Old marinade seasoning 120g</t>
+        </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -1290,7 +1290,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>005. 道地-蘋果綠茶 500ml</t>
+          <t>道地-蘋果綠茶 500ml</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -1309,21 +1309,21 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>697-6901700001</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>005. Authentic-Apple Green Tea 500ml</t>
-        </is>
-      </c>
-      <c r="J21" t="n">
-        <v>27.68</v>
+          <t>6976901700001</t>
+        </is>
+      </c>
+      <c r="I21" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Authentic-apple green tea 500ml</t>
+        </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -1332,7 +1332,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>006. 道地-巨峰紅茶 500ml</t>
+          <t>道地-巨峰紅茶 500ml</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -1351,21 +1351,21 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>697-6901700018</t>
-        </is>
-      </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>006. Authentic-Jufeng black tea 500ml</t>
-        </is>
-      </c>
-      <c r="J22" t="n">
-        <v>27.68</v>
+          <t>6976901700018</t>
+        </is>
+      </c>
+      <c r="I22" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>Authentic-Jufeng Black Tea 500ml</t>
+        </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -1374,7 +1374,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>007. Calpis 原味可爾必思 990ml</t>
+          <t>Calpis 原味可爾必思 990ml</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -1393,21 +1393,21 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>471-4947001131</t>
-        </is>
-      </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>007. Calpis original flavor Kerbes 990ml</t>
-        </is>
-      </c>
-      <c r="J23" t="n">
-        <v>32.46</v>
+          <t>4714947001131</t>
+        </is>
+      </c>
+      <c r="I23" t="n">
+        <v>2.71</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>Calpis Original Calle Betis 990ml</t>
+        </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -1416,7 +1416,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>008. Calpis 原味可爾必思 500ml</t>
+          <t>Calpis 原味可爾必思 500ml</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -1435,21 +1435,21 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>471-4947000134</t>
-        </is>
-      </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>008. Calpis original flavor Kerbes 500ml</t>
-        </is>
-      </c>
-      <c r="J24" t="n">
-        <v>38.18</v>
+          <t>4714947000134</t>
+        </is>
+      </c>
+      <c r="I24" t="n">
+        <v>1.59</v>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>Calpis original flavor Kerbis Betis 500ml</t>
+        </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -1458,7 +1458,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>009. Calpis 葡萄可爾必思 500ml</t>
+          <t>Calpis 葡萄可爾必思 500ml</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -1477,21 +1477,21 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>471-4947013615</t>
-        </is>
-      </c>
-      <c r="I25" t="inlineStr">
-        <is>
-          <t>009. Calpis Grape Calbin 500ml</t>
-        </is>
-      </c>
-      <c r="J25" t="n">
-        <v>38.18</v>
+          <t>4714947013615</t>
+        </is>
+      </c>
+      <c r="I25" t="n">
+        <v>1.59</v>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>Calpis Grape Calbin 500ml</t>
+        </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -1500,7 +1500,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>013. 成央記-海南老椰汁 420ml</t>
+          <t>成央記-海南老椰汁 420ml</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -1519,21 +1519,21 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>697-2698570087</t>
-        </is>
-      </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>013. Cheng Yangji-Hainan Old Coconut Sprace</t>
-        </is>
-      </c>
-      <c r="J26" t="n">
-        <v>92.40000000000001</v>
+          <t>6972698570087</t>
+        </is>
+      </c>
+      <c r="I26" t="n">
+        <v>3.85</v>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>Cheng Yang Ji-Hainan Old Coconut Sprathy 420ml</t>
+        </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -1542,7 +1542,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>014. 道地-烏龍茶 500ml</t>
+          <t>道地-烏龍茶 500ml</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -1561,21 +1561,21 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>693-0599700026</t>
-        </is>
-      </c>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>014. Authentic-oolong tea 500ml</t>
-        </is>
-      </c>
-      <c r="J27" t="n">
-        <v>13.84</v>
+          <t>6930599700026</t>
+        </is>
+      </c>
+      <c r="I27" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>Authentic-oolong tea 500ml</t>
+        </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -1584,7 +1584,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>015. 道地-解。綠茶 500ml</t>
+          <t>道地-解。綠茶 500ml</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -1603,16 +1603,16 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>693-0599700101</t>
-        </is>
-      </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>015. Authentic-solution.Green Tea 500ml</t>
-        </is>
-      </c>
-      <c r="J28" t="n">
-        <v>13.84</v>
+          <t>6930599700101</t>
+        </is>
+      </c>
+      <c r="I28" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>Authentic-solution.Green Tea 500ml</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>